<commit_message>
Add test cases for Memory class
</commit_message>
<xml_diff>
--- a/Test document/OSSimulator test case.xlsx.xlsx
+++ b/Test document/OSSimulator test case.xlsx.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_Projects\OSSimulator\Test document\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="12435" windowHeight="6990" activeTab="4"/>
+    <workbookView xWindow="120" yWindow="30" windowWidth="12435" windowHeight="6990" tabRatio="572" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Test classification" sheetId="2" r:id="rId1"/>
@@ -15,12 +20,12 @@
     <sheet name="Timer" sheetId="6" r:id="rId6"/>
     <sheet name="Utils" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="77">
   <si>
     <t>No</t>
   </si>
@@ -162,6 +167,133 @@
 1
 99
 =&gt; load success</t>
+  </si>
+  <si>
+    <t>Initialize with input array has size &gt; 2000</t>
+  </si>
+  <si>
+    <t>input array has 2001 elements
+=&gt; Error "Exceed maximum memory" display =&gt; Exit</t>
+  </si>
+  <si>
+    <t>Initialize with input array has size &lt; 2000</t>
+  </si>
+  <si>
+    <t>Initialize with input array has size = 2000</t>
+  </si>
+  <si>
+    <t>Input array has 2000 elements
+=&gt; Initialize success</t>
+  </si>
+  <si>
+    <t>input array has 1 elements
+=&gt; Error "Does not meet minimum requirement of memory" display =&gt; Exit</t>
+  </si>
+  <si>
+    <t>Current mode is User (1).
+After switch, current mode is System (2)</t>
+  </si>
+  <si>
+    <t>Current mode is System (2).
+After switch, current mode is User (1)</t>
+  </si>
+  <si>
+    <t>Switch from User -&gt; System</t>
+  </si>
+  <si>
+    <t>Switch from System -&gt; User</t>
+  </si>
+  <si>
+    <t>Read - User program access system memory</t>
+  </si>
+  <si>
+    <t>- Mode: 1
+- Access address: 1000
+-&gt; Error: "Access error" display =&gt; Exit</t>
+  </si>
+  <si>
+    <t>Read - Access address less than 0</t>
+  </si>
+  <si>
+    <t>- Access address: -1
+-&gt; Error: "Invalid address" display =&gt; Exit</t>
+  </si>
+  <si>
+    <t>Read - Access address greater than 2000</t>
+  </si>
+  <si>
+    <t>- Access address: 2001
+-&gt; Error: "Invalid address" display =&gt; Exit</t>
+  </si>
+  <si>
+    <t>Read - User program read memory</t>
+  </si>
+  <si>
+    <t>- Mode: 1
+- Access address: 10; memory[10] = 5
+-&gt; Return 5.</t>
+  </si>
+  <si>
+    <t>Read - system access user memory</t>
+  </si>
+  <si>
+    <t>- Mode: 2
+- Access address: 999
+-&gt; Error: "Access error" display =&gt; Exit</t>
+  </si>
+  <si>
+    <t>- Mode: 2
+- Access address: 1999; memory[1999] = 1;
+-&gt; Return 1</t>
+  </si>
+  <si>
+    <t>Write - User program write data to system memory</t>
+  </si>
+  <si>
+    <t>- Mode: 1
+- Address: 1000; data: 1
+-&gt; Error: "Access error" display =&gt; Exit</t>
+  </si>
+  <si>
+    <t>Write - Access address less than 0</t>
+  </si>
+  <si>
+    <t>Write - Access address greater than 2000</t>
+  </si>
+  <si>
+    <t>Write - User program write data &lt; 0 to memory</t>
+  </si>
+  <si>
+    <t>- Mode: 1
+- Access address: 10; memory[10] = -1
+-&gt; Error: "Invalid data" display =&gt; Exit</t>
+  </si>
+  <si>
+    <t>Write - User program write data to memory</t>
+  </si>
+  <si>
+    <t>- Mode: 1
+- Access address: 999, data: 1
+- &gt; memory[999] = 1</t>
+  </si>
+  <si>
+    <t>Write - Systen write data to user memory</t>
+  </si>
+  <si>
+    <t>Read - System read memory</t>
+  </si>
+  <si>
+    <t>- Mode: 2
+- Access address: 999; data = 1
+-&gt; Error: "Access error" display =&gt; Exit</t>
+  </si>
+  <si>
+    <t>Write - Systen write data</t>
+  </si>
+  <si>
+    <t>- Mode: 2
+- Access address: 1999; data = 1
+- &gt; memory[1999] = 1</t>
   </si>
 </sst>
 </file>
@@ -252,7 +384,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -271,6 +403,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -332,7 +470,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -367,7 +505,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -579,7 +717,7 @@
   <dimension ref="B3:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -715,14 +853,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.28515625" customWidth="1"/>
-    <col min="2" max="2" width="28.7109375" customWidth="1"/>
+    <col min="2" max="2" width="39" customWidth="1"/>
     <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="67.140625" customWidth="1"/>
   </cols>
@@ -766,188 +904,292 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <f>IF(C7&lt;&gt;"",COUNTA($C$6:C6),"")</f>
         <v>1</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" s="9" t="s">
+        <v>43</v>
+      </c>
       <c r="C7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="1"/>
+        <v>22</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <f>IF(C8&lt;&gt;"",COUNTA($C$6:C7),"")</f>
         <v>2</v>
       </c>
-      <c r="B8" s="2"/>
+      <c r="B8" s="9" t="s">
+        <v>45</v>
+      </c>
       <c r="C8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="1"/>
+      <c r="D8" s="4" t="s">
+        <v>48</v>
+      </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="str">
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
         <f>IF(C9&lt;&gt;"",COUNTA($C$6:C8),"")</f>
-        <v/>
-      </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>47</v>
+      </c>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="str">
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
         <f>IF(C10&lt;&gt;"",COUNTA($C$6:C9),"")</f>
-        <v/>
-      </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="str">
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
         <f>IF(C11&lt;&gt;"",COUNTA($C$6:C10),"")</f>
-        <v/>
-      </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
+        <v>5</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="str">
+    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
         <f>IF(C12&lt;&gt;"",COUNTA($C$6:C11),"")</f>
-        <v/>
-      </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>54</v>
+      </c>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="str">
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
         <f>IF(C13&lt;&gt;"",COUNTA($C$6:C12),"")</f>
-        <v/>
-      </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>56</v>
+      </c>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="str">
+    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
         <f>IF(C14&lt;&gt;"",COUNTA($C$6:C13),"")</f>
-        <v/>
-      </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
+        <v>8</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>58</v>
+      </c>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="str">
+    <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
         <f>IF(C15&lt;&gt;"",COUNTA($C$6:C14),"")</f>
-        <v/>
-      </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>60</v>
+      </c>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="str">
+    <row r="16" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
         <f>IF(C16&lt;&gt;"",COUNTA($C$6:C15),"")</f>
-        <v/>
-      </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>62</v>
+      </c>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="str">
+    <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
         <f>IF(C17&lt;&gt;"",COUNTA($C$6:C16),"")</f>
-        <v/>
-      </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
+        <v>11</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>63</v>
+      </c>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="str">
+    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
         <f>IF(C18&lt;&gt;"",COUNTA($C$6:C17),"")</f>
-        <v/>
-      </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
+        <v>12</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>65</v>
+      </c>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="str">
+    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
         <f>IF(C19&lt;&gt;"",COUNTA($C$6:C18),"")</f>
-        <v/>
-      </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
+        <v>13</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>56</v>
+      </c>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="str">
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
         <f>IF(C20&lt;&gt;"",COUNTA($C$6:C19),"")</f>
-        <v/>
-      </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>58</v>
+      </c>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="str">
+    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
         <f>IF(C21&lt;&gt;"",COUNTA($C$6:C20),"")</f>
-        <v/>
-      </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
+        <v>15</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>69</v>
+      </c>
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="str">
+    <row r="22" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
         <f>IF(C22&lt;&gt;"",COUNTA($C$6:C21),"")</f>
-        <v/>
-      </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
+        <v>16</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>71</v>
+      </c>
       <c r="E22" s="1"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="str">
+    <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
         <f>IF(C23&lt;&gt;"",COUNTA($C$6:C22),"")</f>
-        <v/>
-      </c>
-      <c r="B23" s="2"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
+        <v>17</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>74</v>
+      </c>
       <c r="E23" s="1"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="str">
+    <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
         <f>IF(C24&lt;&gt;"",COUNTA($C$6:C23),"")</f>
-        <v/>
-      </c>
-      <c r="B24" s="2"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
+        <v>18</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>76</v>
+      </c>
       <c r="E24" s="1"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -955,7 +1197,7 @@
         <f>IF(C25&lt;&gt;"",COUNTA($C$6:C24),"")</f>
         <v/>
       </c>
-      <c r="B25" s="2"/>
+      <c r="B25" s="9"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
@@ -965,7 +1207,7 @@
         <f>IF(C26&lt;&gt;"",COUNTA($C$6:C25),"")</f>
         <v/>
       </c>
-      <c r="B26" s="2"/>
+      <c r="B26" s="9"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
@@ -975,7 +1217,7 @@
         <f>IF(C27&lt;&gt;"",COUNTA($C$6:C26),"")</f>
         <v/>
       </c>
-      <c r="B27" s="2"/>
+      <c r="B27" s="9"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
@@ -985,7 +1227,7 @@
         <f>IF(C28&lt;&gt;"",COUNTA($C$6:C27),"")</f>
         <v/>
       </c>
-      <c r="B28" s="2"/>
+      <c r="B28" s="9"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
@@ -995,7 +1237,7 @@
         <f>IF(C29&lt;&gt;"",COUNTA($C$6:C28),"")</f>
         <v/>
       </c>
-      <c r="B29" s="2"/>
+      <c r="B29" s="9"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
@@ -1005,7 +1247,7 @@
         <f>IF(C30&lt;&gt;"",COUNTA($C$6:C29),"")</f>
         <v/>
       </c>
-      <c r="B30" s="2"/>
+      <c r="B30" s="9"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
@@ -1015,7 +1257,7 @@
         <f>IF(C31&lt;&gt;"",COUNTA($C$6:C30),"")</f>
         <v/>
       </c>
-      <c r="B31" s="2"/>
+      <c r="B31" s="9"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
@@ -1025,7 +1267,7 @@
         <f>IF(C32&lt;&gt;"",COUNTA($C$6:C31),"")</f>
         <v/>
       </c>
-      <c r="B32" s="2"/>
+      <c r="B32" s="9"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
@@ -1035,7 +1277,7 @@
         <f>IF(C33&lt;&gt;"",COUNTA($C$6:C32),"")</f>
         <v/>
       </c>
-      <c r="B33" s="2"/>
+      <c r="B33" s="9"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
@@ -1045,7 +1287,7 @@
         <f>IF(C34&lt;&gt;"",COUNTA($C$6:C33),"")</f>
         <v/>
       </c>
-      <c r="B34" s="2"/>
+      <c r="B34" s="9"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
@@ -1055,7 +1297,7 @@
         <f>IF(C35&lt;&gt;"",COUNTA($C$6:C34),"")</f>
         <v/>
       </c>
-      <c r="B35" s="2"/>
+      <c r="B35" s="9"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
@@ -1065,7 +1307,7 @@
         <f>IF(C36&lt;&gt;"",COUNTA($C$6:C35),"")</f>
         <v/>
       </c>
-      <c r="B36" s="2"/>
+      <c r="B36" s="9"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
@@ -1075,7 +1317,7 @@
         <f>IF(C37&lt;&gt;"",COUNTA($C$6:C36),"")</f>
         <v/>
       </c>
-      <c r="B37" s="2"/>
+      <c r="B37" s="9"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
@@ -1085,7 +1327,7 @@
         <f>IF(C38&lt;&gt;"",COUNTA($C$6:C37),"")</f>
         <v/>
       </c>
-      <c r="B38" s="2"/>
+      <c r="B38" s="9"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
@@ -1095,7 +1337,7 @@
         <f>IF(C39&lt;&gt;"",COUNTA($C$6:C38),"")</f>
         <v/>
       </c>
-      <c r="B39" s="2"/>
+      <c r="B39" s="9"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
@@ -1105,7 +1347,7 @@
         <f>IF(C40&lt;&gt;"",COUNTA($C$6:C39),"")</f>
         <v/>
       </c>
-      <c r="B40" s="2"/>
+      <c r="B40" s="9"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
@@ -1115,7 +1357,7 @@
         <f>IF(C41&lt;&gt;"",COUNTA($C$6:C40),"")</f>
         <v/>
       </c>
-      <c r="B41" s="2"/>
+      <c r="B41" s="9"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
@@ -1125,7 +1367,7 @@
         <f>IF(C42&lt;&gt;"",COUNTA($C$6:C41),"")</f>
         <v/>
       </c>
-      <c r="B42" s="2"/>
+      <c r="B42" s="9"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
@@ -1135,7 +1377,7 @@
         <f>IF(C43&lt;&gt;"",COUNTA($C$6:C42),"")</f>
         <v/>
       </c>
-      <c r="B43" s="2"/>
+      <c r="B43" s="9"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
@@ -1145,7 +1387,7 @@
         <f>IF(C44&lt;&gt;"",COUNTA($C$6:C43),"")</f>
         <v/>
       </c>
-      <c r="B44" s="2"/>
+      <c r="B44" s="9"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
@@ -1155,7 +1397,7 @@
         <f>IF(C45&lt;&gt;"",COUNTA($C$6:C44),"")</f>
         <v/>
       </c>
-      <c r="B45" s="2"/>
+      <c r="B45" s="9"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
@@ -1165,7 +1407,7 @@
         <f>IF(C46&lt;&gt;"",COUNTA($C$6:C45),"")</f>
         <v/>
       </c>
-      <c r="B46" s="2"/>
+      <c r="B46" s="9"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
@@ -1175,7 +1417,7 @@
         <f>IF(C47&lt;&gt;"",COUNTA($C$6:C46),"")</f>
         <v/>
       </c>
-      <c r="B47" s="2"/>
+      <c r="B47" s="9"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
@@ -1185,7 +1427,7 @@
         <f>IF(C48&lt;&gt;"",COUNTA($C$6:C47),"")</f>
         <v/>
       </c>
-      <c r="B48" s="2"/>
+      <c r="B48" s="9"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
@@ -1195,7 +1437,7 @@
         <f>IF(C49&lt;&gt;"",COUNTA($C$6:C48),"")</f>
         <v/>
       </c>
-      <c r="B49" s="2"/>
+      <c r="B49" s="9"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
@@ -1205,7 +1447,7 @@
         <f>IF(C50&lt;&gt;"",COUNTA($C$6:C49),"")</f>
         <v/>
       </c>
-      <c r="B50" s="2"/>
+      <c r="B50" s="9"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
@@ -1215,7 +1457,7 @@
         <f>IF(C51&lt;&gt;"",COUNTA($C$6:C50),"")</f>
         <v/>
       </c>
-      <c r="B51" s="2"/>
+      <c r="B51" s="9"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
@@ -1225,7 +1467,7 @@
         <f>IF(C52&lt;&gt;"",COUNTA($C$6:C51),"")</f>
         <v/>
       </c>
-      <c r="B52" s="2"/>
+      <c r="B52" s="9"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
@@ -1235,7 +1477,7 @@
         <f>IF(C53&lt;&gt;"",COUNTA($C$6:C52),"")</f>
         <v/>
       </c>
-      <c r="B53" s="2"/>
+      <c r="B53" s="9"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
@@ -1245,7 +1487,7 @@
         <f>IF(C54&lt;&gt;"",COUNTA($C$6:C53),"")</f>
         <v/>
       </c>
-      <c r="B54" s="2"/>
+      <c r="B54" s="9"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
@@ -1255,7 +1497,7 @@
         <f>IF(C55&lt;&gt;"",COUNTA($C$6:C54),"")</f>
         <v/>
       </c>
-      <c r="B55" s="2"/>
+      <c r="B55" s="9"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
@@ -1265,7 +1507,7 @@
         <f>IF(C56&lt;&gt;"",COUNTA($C$6:C55),"")</f>
         <v/>
       </c>
-      <c r="B56" s="2"/>
+      <c r="B56" s="9"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
@@ -1275,7 +1517,7 @@
         <f>IF(C57&lt;&gt;"",COUNTA($C$6:C56),"")</f>
         <v/>
       </c>
-      <c r="B57" s="2"/>
+      <c r="B57" s="9"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
@@ -1285,7 +1527,7 @@
         <f>IF(C58&lt;&gt;"",COUNTA($C$6:C57),"")</f>
         <v/>
       </c>
-      <c r="B58" s="2"/>
+      <c r="B58" s="9"/>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
@@ -1295,7 +1537,7 @@
         <f>IF(C59&lt;&gt;"",COUNTA($C$6:C58),"")</f>
         <v/>
       </c>
-      <c r="B59" s="2"/>
+      <c r="B59" s="9"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
@@ -2780,7 +3022,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
@@ -3810,7 +4052,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Implement instructions 21 - 30
</commit_message>
<xml_diff>
--- a/Test document/OSSimulator test case.xlsx.xlsx
+++ b/Test document/OSSimulator test case.xlsx.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JavaPrjs\OSSimulator\Test document\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="12435" windowHeight="6990" activeTab="4"/>
+    <workbookView xWindow="120" yWindow="30" windowWidth="12435" windowHeight="6990" tabRatio="572" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test classification" sheetId="2" r:id="rId1"/>
@@ -15,12 +20,12 @@
     <sheet name="Timer" sheetId="6" r:id="rId6"/>
     <sheet name="Utils" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="71">
   <si>
     <t>No</t>
   </si>
@@ -162,6 +167,109 @@
 1
 99
 =&gt; load success</t>
+  </si>
+  <si>
+    <t>Initialize with input array has size &gt; 2000</t>
+  </si>
+  <si>
+    <t>input array has 2001 elements
+=&gt; Error "Exceed maximum memory" display =&gt; Exit</t>
+  </si>
+  <si>
+    <t>Initialize with input array has size &lt; 2000</t>
+  </si>
+  <si>
+    <t>Initialize with input array has size = 2000</t>
+  </si>
+  <si>
+    <t>Input array has 2000 elements
+=&gt; Initialize success</t>
+  </si>
+  <si>
+    <t>input array has 1 elements
+=&gt; Error "Does not meet minimum requirement of memory" display =&gt; Exit</t>
+  </si>
+  <si>
+    <t>Current mode is User (1).
+After switch, current mode is System (2)</t>
+  </si>
+  <si>
+    <t>Current mode is System (2).
+After switch, current mode is User (1)</t>
+  </si>
+  <si>
+    <t>Switch from User -&gt; System</t>
+  </si>
+  <si>
+    <t>Switch from System -&gt; User</t>
+  </si>
+  <si>
+    <t>Read - User program access system memory</t>
+  </si>
+  <si>
+    <t>- Mode: 1
+- Access address: 1000
+-&gt; Error: "Access error" display =&gt; Exit</t>
+  </si>
+  <si>
+    <t>Read - Access address less than 0</t>
+  </si>
+  <si>
+    <t>- Access address: -1
+-&gt; Error: "Invalid address" display =&gt; Exit</t>
+  </si>
+  <si>
+    <t>Read - Access address greater than 2000</t>
+  </si>
+  <si>
+    <t>- Access address: 2001
+-&gt; Error: "Invalid address" display =&gt; Exit</t>
+  </si>
+  <si>
+    <t>Read - User program read memory</t>
+  </si>
+  <si>
+    <t>- Mode: 1
+- Access address: 10; memory[10] = 5
+-&gt; Return 5.</t>
+  </si>
+  <si>
+    <t>- Mode: 2
+- Access address: 1999; memory[1999] = 1;
+-&gt; Return 1</t>
+  </si>
+  <si>
+    <t>Write - User program write data to system memory</t>
+  </si>
+  <si>
+    <t>- Mode: 1
+- Address: 1000; data: 1
+-&gt; Error: "Access error" display =&gt; Exit</t>
+  </si>
+  <si>
+    <t>Write - Access address less than 0</t>
+  </si>
+  <si>
+    <t>Write - Access address greater than 2000</t>
+  </si>
+  <si>
+    <t>Write - User program write data to memory</t>
+  </si>
+  <si>
+    <t>- Mode: 1
+- Access address: 999, data: 1
+- &gt; memory[999] = 1</t>
+  </si>
+  <si>
+    <t>Read - System read memory</t>
+  </si>
+  <si>
+    <t>Write - Systen write data</t>
+  </si>
+  <si>
+    <t>- Mode: 2
+- Access address: 1999; data = 1
+- &gt; memory[1999] = 1</t>
   </si>
 </sst>
 </file>
@@ -252,7 +360,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -264,6 +372,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -332,7 +446,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -367,7 +481,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -579,7 +693,7 @@
   <dimension ref="B3:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -713,22 +827,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G101"/>
+  <dimension ref="A2:G98"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.28515625" customWidth="1"/>
-    <col min="2" max="2" width="28.7109375" customWidth="1"/>
+    <col min="2" max="2" width="39" customWidth="1"/>
     <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="67.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="9" t="s">
         <v>14</v>
       </c>
       <c r="F2" s="3" t="s">
@@ -739,13 +853,13 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E3" s="8"/>
+      <c r="E3" s="10"/>
       <c r="F3" s="1">
-        <f>COUNTIF(E7:E345,"OK")</f>
+        <f>COUNTIF(E7:E342,"OK")</f>
         <v>0</v>
       </c>
       <c r="G3" s="1">
-        <f>COUNTIF(E7:E345,"NG")</f>
+        <f>COUNTIF(E7:E342,"NG")</f>
         <v>0</v>
       </c>
     </row>
@@ -766,158 +880,244 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <f>IF(C7&lt;&gt;"",COUNTA($C$6:C6),"")</f>
         <v>1</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" s="7" t="s">
+        <v>43</v>
+      </c>
       <c r="C7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="1"/>
+        <v>22</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <f>IF(C8&lt;&gt;"",COUNTA($C$6:C7),"")</f>
         <v>2</v>
       </c>
-      <c r="B8" s="2"/>
+      <c r="B8" s="7" t="s">
+        <v>45</v>
+      </c>
       <c r="C8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="1"/>
+      <c r="D8" s="4" t="s">
+        <v>48</v>
+      </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="str">
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
         <f>IF(C9&lt;&gt;"",COUNTA($C$6:C8),"")</f>
-        <v/>
-      </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>47</v>
+      </c>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="str">
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
         <f>IF(C10&lt;&gt;"",COUNTA($C$6:C9),"")</f>
-        <v/>
-      </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="str">
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
         <f>IF(C11&lt;&gt;"",COUNTA($C$6:C10),"")</f>
-        <v/>
-      </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
+        <v>5</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="str">
+    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
         <f>IF(C12&lt;&gt;"",COUNTA($C$6:C11),"")</f>
-        <v/>
-      </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>54</v>
+      </c>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="str">
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
         <f>IF(C13&lt;&gt;"",COUNTA($C$6:C12),"")</f>
-        <v/>
-      </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>56</v>
+      </c>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="str">
+    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
         <f>IF(C14&lt;&gt;"",COUNTA($C$6:C13),"")</f>
-        <v/>
-      </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
+        <v>8</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>58</v>
+      </c>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="str">
+    <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
         <f>IF(C15&lt;&gt;"",COUNTA($C$6:C14),"")</f>
-        <v/>
-      </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>60</v>
+      </c>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="str">
+    <row r="16" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
         <f>IF(C16&lt;&gt;"",COUNTA($C$6:C15),"")</f>
-        <v/>
-      </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>61</v>
+      </c>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="str">
+    <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
         <f>IF(C17&lt;&gt;"",COUNTA($C$6:C16),"")</f>
-        <v/>
-      </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
+        <v>11</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>63</v>
+      </c>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="str">
+    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
         <f>IF(C18&lt;&gt;"",COUNTA($C$6:C17),"")</f>
-        <v/>
-      </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
+        <v>12</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>56</v>
+      </c>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="str">
+    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
         <f>IF(C19&lt;&gt;"",COUNTA($C$6:C18),"")</f>
-        <v/>
-      </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
+        <v>13</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>58</v>
+      </c>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="str">
+    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
         <f>IF(C20&lt;&gt;"",COUNTA($C$6:C19),"")</f>
-        <v/>
-      </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>67</v>
+      </c>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="str">
+    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
         <f>IF(C21&lt;&gt;"",COUNTA($C$6:C20),"")</f>
-        <v/>
-      </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
+        <v>15</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>70</v>
+      </c>
       <c r="E21" s="1"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -925,7 +1125,7 @@
         <f>IF(C22&lt;&gt;"",COUNTA($C$6:C21),"")</f>
         <v/>
       </c>
-      <c r="B22" s="2"/>
+      <c r="B22" s="7"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -935,7 +1135,7 @@
         <f>IF(C23&lt;&gt;"",COUNTA($C$6:C22),"")</f>
         <v/>
       </c>
-      <c r="B23" s="2"/>
+      <c r="B23" s="7"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -945,7 +1145,7 @@
         <f>IF(C24&lt;&gt;"",COUNTA($C$6:C23),"")</f>
         <v/>
       </c>
-      <c r="B24" s="2"/>
+      <c r="B24" s="7"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
@@ -955,7 +1155,7 @@
         <f>IF(C25&lt;&gt;"",COUNTA($C$6:C24),"")</f>
         <v/>
       </c>
-      <c r="B25" s="2"/>
+      <c r="B25" s="7"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
@@ -965,7 +1165,7 @@
         <f>IF(C26&lt;&gt;"",COUNTA($C$6:C25),"")</f>
         <v/>
       </c>
-      <c r="B26" s="2"/>
+      <c r="B26" s="7"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
@@ -975,7 +1175,7 @@
         <f>IF(C27&lt;&gt;"",COUNTA($C$6:C26),"")</f>
         <v/>
       </c>
-      <c r="B27" s="2"/>
+      <c r="B27" s="7"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
@@ -985,7 +1185,7 @@
         <f>IF(C28&lt;&gt;"",COUNTA($C$6:C27),"")</f>
         <v/>
       </c>
-      <c r="B28" s="2"/>
+      <c r="B28" s="7"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
@@ -995,7 +1195,7 @@
         <f>IF(C29&lt;&gt;"",COUNTA($C$6:C28),"")</f>
         <v/>
       </c>
-      <c r="B29" s="2"/>
+      <c r="B29" s="7"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
@@ -1005,7 +1205,7 @@
         <f>IF(C30&lt;&gt;"",COUNTA($C$6:C29),"")</f>
         <v/>
       </c>
-      <c r="B30" s="2"/>
+      <c r="B30" s="7"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
@@ -1015,7 +1215,7 @@
         <f>IF(C31&lt;&gt;"",COUNTA($C$6:C30),"")</f>
         <v/>
       </c>
-      <c r="B31" s="2"/>
+      <c r="B31" s="7"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
@@ -1025,7 +1225,7 @@
         <f>IF(C32&lt;&gt;"",COUNTA($C$6:C31),"")</f>
         <v/>
       </c>
-      <c r="B32" s="2"/>
+      <c r="B32" s="7"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
@@ -1035,7 +1235,7 @@
         <f>IF(C33&lt;&gt;"",COUNTA($C$6:C32),"")</f>
         <v/>
       </c>
-      <c r="B33" s="2"/>
+      <c r="B33" s="7"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
@@ -1045,7 +1245,7 @@
         <f>IF(C34&lt;&gt;"",COUNTA($C$6:C33),"")</f>
         <v/>
       </c>
-      <c r="B34" s="2"/>
+      <c r="B34" s="7"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
@@ -1055,7 +1255,7 @@
         <f>IF(C35&lt;&gt;"",COUNTA($C$6:C34),"")</f>
         <v/>
       </c>
-      <c r="B35" s="2"/>
+      <c r="B35" s="7"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
@@ -1065,7 +1265,7 @@
         <f>IF(C36&lt;&gt;"",COUNTA($C$6:C35),"")</f>
         <v/>
       </c>
-      <c r="B36" s="2"/>
+      <c r="B36" s="7"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
@@ -1075,7 +1275,7 @@
         <f>IF(C37&lt;&gt;"",COUNTA($C$6:C36),"")</f>
         <v/>
       </c>
-      <c r="B37" s="2"/>
+      <c r="B37" s="7"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
@@ -1085,7 +1285,7 @@
         <f>IF(C38&lt;&gt;"",COUNTA($C$6:C37),"")</f>
         <v/>
       </c>
-      <c r="B38" s="2"/>
+      <c r="B38" s="7"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
@@ -1095,7 +1295,7 @@
         <f>IF(C39&lt;&gt;"",COUNTA($C$6:C38),"")</f>
         <v/>
       </c>
-      <c r="B39" s="2"/>
+      <c r="B39" s="7"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
@@ -1105,7 +1305,7 @@
         <f>IF(C40&lt;&gt;"",COUNTA($C$6:C39),"")</f>
         <v/>
       </c>
-      <c r="B40" s="2"/>
+      <c r="B40" s="7"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
@@ -1115,7 +1315,7 @@
         <f>IF(C41&lt;&gt;"",COUNTA($C$6:C40),"")</f>
         <v/>
       </c>
-      <c r="B41" s="2"/>
+      <c r="B41" s="7"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
@@ -1125,7 +1325,7 @@
         <f>IF(C42&lt;&gt;"",COUNTA($C$6:C41),"")</f>
         <v/>
       </c>
-      <c r="B42" s="2"/>
+      <c r="B42" s="7"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
@@ -1135,7 +1335,7 @@
         <f>IF(C43&lt;&gt;"",COUNTA($C$6:C42),"")</f>
         <v/>
       </c>
-      <c r="B43" s="2"/>
+      <c r="B43" s="7"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
@@ -1145,7 +1345,7 @@
         <f>IF(C44&lt;&gt;"",COUNTA($C$6:C43),"")</f>
         <v/>
       </c>
-      <c r="B44" s="2"/>
+      <c r="B44" s="7"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
@@ -1155,7 +1355,7 @@
         <f>IF(C45&lt;&gt;"",COUNTA($C$6:C44),"")</f>
         <v/>
       </c>
-      <c r="B45" s="2"/>
+      <c r="B45" s="7"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
@@ -1165,7 +1365,7 @@
         <f>IF(C46&lt;&gt;"",COUNTA($C$6:C45),"")</f>
         <v/>
       </c>
-      <c r="B46" s="2"/>
+      <c r="B46" s="7"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
@@ -1175,7 +1375,7 @@
         <f>IF(C47&lt;&gt;"",COUNTA($C$6:C46),"")</f>
         <v/>
       </c>
-      <c r="B47" s="2"/>
+      <c r="B47" s="7"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
@@ -1185,7 +1385,7 @@
         <f>IF(C48&lt;&gt;"",COUNTA($C$6:C47),"")</f>
         <v/>
       </c>
-      <c r="B48" s="2"/>
+      <c r="B48" s="7"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
@@ -1195,7 +1395,7 @@
         <f>IF(C49&lt;&gt;"",COUNTA($C$6:C48),"")</f>
         <v/>
       </c>
-      <c r="B49" s="2"/>
+      <c r="B49" s="7"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
@@ -1205,7 +1405,7 @@
         <f>IF(C50&lt;&gt;"",COUNTA($C$6:C49),"")</f>
         <v/>
       </c>
-      <c r="B50" s="2"/>
+      <c r="B50" s="7"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
@@ -1215,7 +1415,7 @@
         <f>IF(C51&lt;&gt;"",COUNTA($C$6:C50),"")</f>
         <v/>
       </c>
-      <c r="B51" s="2"/>
+      <c r="B51" s="7"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
@@ -1225,7 +1425,7 @@
         <f>IF(C52&lt;&gt;"",COUNTA($C$6:C51),"")</f>
         <v/>
       </c>
-      <c r="B52" s="2"/>
+      <c r="B52" s="7"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
@@ -1235,7 +1435,7 @@
         <f>IF(C53&lt;&gt;"",COUNTA($C$6:C52),"")</f>
         <v/>
       </c>
-      <c r="B53" s="2"/>
+      <c r="B53" s="7"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
@@ -1245,7 +1445,7 @@
         <f>IF(C54&lt;&gt;"",COUNTA($C$6:C53),"")</f>
         <v/>
       </c>
-      <c r="B54" s="2"/>
+      <c r="B54" s="7"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
@@ -1255,7 +1455,7 @@
         <f>IF(C55&lt;&gt;"",COUNTA($C$6:C54),"")</f>
         <v/>
       </c>
-      <c r="B55" s="2"/>
+      <c r="B55" s="7"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
@@ -1265,7 +1465,7 @@
         <f>IF(C56&lt;&gt;"",COUNTA($C$6:C55),"")</f>
         <v/>
       </c>
-      <c r="B56" s="2"/>
+      <c r="B56" s="7"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
@@ -1689,36 +1889,6 @@
       <c r="C98" s="1"/>
       <c r="D98" s="1"/>
       <c r="E98" s="1"/>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A99" s="2" t="str">
-        <f>IF(C99&lt;&gt;"",COUNTA($C$6:C98),"")</f>
-        <v/>
-      </c>
-      <c r="B99" s="2"/>
-      <c r="C99" s="1"/>
-      <c r="D99" s="1"/>
-      <c r="E99" s="1"/>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A100" s="2" t="str">
-        <f>IF(C100&lt;&gt;"",COUNTA($C$6:C99),"")</f>
-        <v/>
-      </c>
-      <c r="B100" s="2"/>
-      <c r="C100" s="1"/>
-      <c r="D100" s="1"/>
-      <c r="E100" s="1"/>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A101" s="2" t="str">
-        <f>IF(C101&lt;&gt;"",COUNTA($C$6:C100),"")</f>
-        <v/>
-      </c>
-      <c r="B101" s="2"/>
-      <c r="C101" s="1"/>
-      <c r="D101" s="1"/>
-      <c r="E101" s="1"/>
     </row>
   </sheetData>
   <dataConsolidate/>
@@ -1726,7 +1896,7 @@
     <mergeCell ref="E2:E3"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E7:E2258">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E7:E2255">
       <formula1>"OK,NG"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1738,7 +1908,7 @@
           <x14:formula1>
             <xm:f>Utils!$B$4:$B$5</xm:f>
           </x14:formula1>
-          <xm:sqref>C7:C101</xm:sqref>
+          <xm:sqref>C7:C98</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1763,7 +1933,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="9" t="s">
         <v>14</v>
       </c>
       <c r="F2" s="3" t="s">
@@ -1774,7 +1944,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E3" s="8"/>
+      <c r="E3" s="10"/>
       <c r="F3" s="1">
         <f>COUNTIF(E7:E345,"OK")</f>
         <v>0</v>
@@ -2793,7 +2963,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="9" t="s">
         <v>14</v>
       </c>
       <c r="F2" s="3" t="s">
@@ -2804,7 +2974,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E3" s="8"/>
+      <c r="E3" s="10"/>
       <c r="F3" s="1">
         <f>COUNTIF(E7:E345,"OK")</f>
         <v>0</v>
@@ -3810,7 +3980,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
@@ -3823,7 +3993,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="9" t="s">
         <v>14</v>
       </c>
       <c r="F2" s="3" t="s">
@@ -3834,7 +4004,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E3" s="8"/>
+      <c r="E3" s="10"/>
       <c r="F3" s="1">
         <f>COUNTIF(E7:E345,"OK")</f>
         <v>0</v>
@@ -4889,7 +5059,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="9" t="s">
         <v>14</v>
       </c>
       <c r="F2" s="3" t="s">
@@ -4900,7 +5070,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E3" s="8"/>
+      <c r="E3" s="10"/>
       <c r="F3" s="1">
         <f>COUNTIF(E7:E345,"OK")</f>
         <v>0</v>

</xml_diff>